<commit_message>
Widened the main text box from 20 to 26 tiles
</commit_message>
<xml_diff>
--- a/psrp/RAM windows cache.xlsx
+++ b/psrp/RAM windows cache.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="146">
   <si>
     <t>What</t>
   </si>
@@ -463,7 +463,10 @@
     <t>Enemy stats (up to 8)</t>
   </si>
   <si>
-    <t>0630</t>
+    <t>0634</t>
+  </si>
+  <si>
+    <t>0330</t>
   </si>
 </sst>
 </file>
@@ -1659,7 +1662,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K3:K24"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1730,19 +1733,19 @@
         <v>108</v>
       </c>
       <c r="G3">
-        <f>HEX2DEC(RIGHT(D3,2))/2</f>
+        <f t="shared" ref="G3:G24" si="0">HEX2DEC(RIGHT(D3,2))/2</f>
         <v>32</v>
       </c>
       <c r="H3">
-        <f>HEX2DEC(LEFT(D3,2))</f>
+        <f t="shared" ref="H3:H24" si="1">HEX2DEC(LEFT(D3,2))</f>
         <v>6</v>
       </c>
       <c r="I3">
-        <f>G3*H3*2</f>
+        <f t="shared" ref="I3:I24" si="2">G3*H3*2</f>
         <v>384</v>
       </c>
       <c r="J3" t="str">
-        <f>DEC2HEX(HEX2DEC(B3)+I3)</f>
+        <f t="shared" ref="J3:J24" si="3">DEC2HEX(HEX2DEC(B3)+I3)</f>
         <v>D880</v>
       </c>
       <c r="K3" t="str">
@@ -1768,23 +1771,23 @@
         <v>100</v>
       </c>
       <c r="G4">
-        <f>HEX2DEC(RIGHT(D4,2))/2</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="H4">
-        <f>HEX2DEC(LEFT(D4,2))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="I4">
-        <f>G4*H4*2</f>
+        <f t="shared" si="2"/>
         <v>384</v>
       </c>
       <c r="J4" t="str">
-        <f>DEC2HEX(HEX2DEC(B4)+I4)</f>
+        <f t="shared" si="3"/>
         <v>D880</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" ref="K4:K24" si="0">"  PatchWindow $"&amp;B4&amp;" $"&amp;LOWER(DEC2HEX(HEX2DEC(A4)+1))&amp;" $"&amp;LOWER(DEC2HEX(HEX2DEC(F4)+1))&amp;" ; "&amp;E4</f>
+        <f t="shared" ref="K4:K24" si="4">"  PatchWindow $"&amp;B4&amp;" $"&amp;LOWER(DEC2HEX(HEX2DEC(A4)+1))&amp;" $"&amp;LOWER(DEC2HEX(HEX2DEC(F4)+1))&amp;" ; "&amp;E4</f>
         <v xml:space="preserve">  PatchWindow $d700 $30fd $1 ; Party stats again</v>
       </c>
     </row>
@@ -1809,23 +1812,23 @@
         <v>110</v>
       </c>
       <c r="G5">
-        <f>HEX2DEC(RIGHT(D5,2))/2</f>
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="H5">
-        <f>HEX2DEC(LEFT(D5,2))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="I5">
-        <f>G5*H5*2</f>
-        <v>288</v>
+        <f t="shared" si="2"/>
+        <v>312</v>
       </c>
       <c r="J5" t="str">
-        <f>DEC2HEX(HEX2DEC(B5)+I5)</f>
-        <v>D9A0</v>
+        <f t="shared" si="3"/>
+        <v>D9B8</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">  PatchWindow $D880 $334d $3587 ; Narrative box</v>
       </c>
     </row>
@@ -1835,13 +1838,13 @@
       </c>
       <c r="B6" t="str">
         <f>J5</f>
-        <v>D9A0</v>
+        <v>D9B8</v>
       </c>
       <c r="C6" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="E6" t="s">
         <v>105</v>
@@ -1850,24 +1853,24 @@
         <v>142</v>
       </c>
       <c r="G6">
-        <f>HEX2DEC(RIGHT(D6,2))/2</f>
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="H6">
-        <f>HEX2DEC(LEFT(D6,2))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I6">
-        <f>G6*H6*2</f>
-        <v>108</v>
+        <f t="shared" si="2"/>
+        <v>144</v>
       </c>
       <c r="J6" t="str">
-        <f>DEC2HEX(HEX2DEC(B6)+I6)</f>
-        <v>DA0C</v>
+        <f t="shared" si="3"/>
+        <v>DA48</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $D9A0 $3554 $3560 ; Narrative box scroll buffer</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $D9B8 $3554 $3560 ; Narrative box scroll buffer</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
@@ -1876,7 +1879,7 @@
       </c>
       <c r="B7" t="str">
         <f>J6</f>
-        <v>DA0C</v>
+        <v>DA48</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>80</v>
@@ -1891,24 +1894,24 @@
         <v>141</v>
       </c>
       <c r="G7">
-        <f>HEX2DEC(RIGHT(D7,2))/2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H7">
-        <f>HEX2DEC(LEFT(D7,2))</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="I7">
-        <f>G7*H7*2</f>
+        <f t="shared" si="2"/>
         <v>176</v>
       </c>
       <c r="J7" t="str">
-        <f>DEC2HEX(HEX2DEC(B7)+I7)</f>
-        <v>DABC</v>
+        <f t="shared" si="3"/>
+        <v>DAF8</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DA0C $322c $324a ; Battle menu</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DA48 $322c $324a ; Battle menu</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
@@ -1917,7 +1920,7 @@
       </c>
       <c r="B8" t="str">
         <f>B7</f>
-        <v>DA0C</v>
+        <v>DA48</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>80</v>
@@ -1932,24 +1935,24 @@
         <v>107</v>
       </c>
       <c r="G8">
-        <f>HEX2DEC(RIGHT(D8,2))/2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H8">
-        <f>HEX2DEC(LEFT(D8,2))</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="I8">
-        <f>G8*H8*2</f>
+        <f t="shared" si="2"/>
         <v>176</v>
       </c>
       <c r="J8" t="str">
-        <f>DEC2HEX(HEX2DEC(B8)+I8)</f>
-        <v>DABC</v>
+        <f t="shared" si="3"/>
+        <v>DAF8</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DA0C $37fb $3819 ; Regular world menu</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DA48 $37fb $3819 ; Regular world menu</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
@@ -1958,7 +1961,7 @@
       </c>
       <c r="B9" t="str">
         <f>B8</f>
-        <v>DA0C</v>
+        <v>DA48</v>
       </c>
       <c r="C9" t="s">
         <v>57</v>
@@ -1973,24 +1976,24 @@
         <v>126</v>
       </c>
       <c r="G9">
-        <f>HEX2DEC(RIGHT(D9,2))/2</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="H9">
-        <f>HEX2DEC(LEFT(D9,2))</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I9">
-        <f>G9*H9*2</f>
+        <f t="shared" si="2"/>
         <v>288</v>
       </c>
       <c r="J9" t="str">
-        <f>DEC2HEX(HEX2DEC(B9)+I9)</f>
-        <v>DB2C</v>
+        <f t="shared" si="3"/>
+        <v>DB68</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DA0C $39eb $3ac4 ; Shop items</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DA48 $39eb $3ac4 ; Shop items</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
@@ -1999,7 +2002,7 @@
       </c>
       <c r="B10" t="str">
         <f>J8</f>
-        <v>DABC</v>
+        <v>DAF8</v>
       </c>
       <c r="C10" t="s">
         <v>49</v>
@@ -2014,24 +2017,24 @@
         <v>117</v>
       </c>
       <c r="G10">
-        <f>HEX2DEC(RIGHT(D10,2))/2</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H10">
-        <f>HEX2DEC(LEFT(D10,2))</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I10">
-        <f>G10*H10*2</f>
+        <f t="shared" si="2"/>
         <v>192</v>
       </c>
       <c r="J10" t="str">
-        <f>DEC2HEX(HEX2DEC(B10)+I10)</f>
-        <v>DB7C</v>
+        <f t="shared" si="3"/>
+        <v>DBB8</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DABC $3826 $386b ; Currently equipped items</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DAF8 $3826 $386b ; Currently equipped items</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
@@ -2040,7 +2043,7 @@
       </c>
       <c r="B11" t="str">
         <f>B10</f>
-        <v>DABC</v>
+        <v>DAF8</v>
       </c>
       <c r="C11" t="s">
         <v>59</v>
@@ -2055,24 +2058,24 @@
         <v>122</v>
       </c>
       <c r="G11">
-        <f>HEX2DEC(RIGHT(D11,2))/2</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H11">
-        <f>HEX2DEC(LEFT(D11,2))</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="I11">
-        <f>G11*H11*2</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="J11" t="str">
-        <f>DEC2HEX(HEX2DEC(B11)+I11)</f>
-        <v>DB94</v>
+        <f t="shared" si="3"/>
+        <v>DBD0</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DABC $3ad0 $3b08 ; Select save slot</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DAF8 $3ad0 $3b08 ; Select save slot</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
@@ -2081,7 +2084,7 @@
       </c>
       <c r="B12" t="str">
         <f>B11</f>
-        <v>DABC</v>
+        <v>DAF8</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>34</v>
@@ -2096,24 +2099,24 @@
         <v>119</v>
       </c>
       <c r="G12">
-        <f>HEX2DEC(RIGHT(D12,2))/2</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H12">
-        <f>HEX2DEC(LEFT(D12,2))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I12">
-        <f>G12*H12*2</f>
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="J12" t="str">
-        <f>DEC2HEX(HEX2DEC(B12)+I12)</f>
-        <v>DB1C</v>
+        <f t="shared" si="3"/>
+        <v>DB58</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DABC $3256 $331b ; Enemy name</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DAF8 $3256 $331b ; Enemy name</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
@@ -2122,7 +2125,7 @@
       </c>
       <c r="B13" t="str">
         <f>B12</f>
-        <v>DABC</v>
+        <v>DAF8</v>
       </c>
       <c r="C13" t="s">
         <v>62</v>
@@ -2137,24 +2140,24 @@
         <v>128</v>
       </c>
       <c r="G13">
-        <f>HEX2DEC(RIGHT(D13,2))/2</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H13">
-        <f>HEX2DEC(LEFT(D13,2))</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I13">
-        <f>G13*H13*2</f>
+        <f t="shared" si="2"/>
         <v>112</v>
       </c>
       <c r="J13" t="str">
-        <f>DEC2HEX(HEX2DEC(B13)+I13)</f>
-        <v>DB2C</v>
+        <f t="shared" si="3"/>
+        <v>DB68</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DABC $3b4c $3b73 ; Hapsby travel</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DAF8 $3b4c $3b73 ; Hapsby travel</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
@@ -2163,7 +2166,7 @@
       </c>
       <c r="B14" t="str">
         <f>J12</f>
-        <v>DB1C</v>
+        <v>DB58</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>83</v>
@@ -2178,24 +2181,24 @@
         <v>120</v>
       </c>
       <c r="G14">
-        <f>HEX2DEC(RIGHT(D14,2))/2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H14">
-        <f>HEX2DEC(LEFT(D14,2))</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I14">
-        <f>G14*H14*2</f>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
       <c r="J14" t="str">
-        <f>DEC2HEX(HEX2DEC(B14)+I14)</f>
-        <v>DBBC</v>
+        <f t="shared" si="3"/>
+        <v>DBF8</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DB1C $3262 $330a ; Enemy stats (up to 8)</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DB58 $3262 $330a ; Enemy stats (up to 8)</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
@@ -2204,7 +2207,7 @@
       </c>
       <c r="B15" t="str">
         <f>J9</f>
-        <v>DB2C</v>
+        <v>DB68</v>
       </c>
       <c r="C15" t="s">
         <v>91</v>
@@ -2219,24 +2222,24 @@
         <v>127</v>
       </c>
       <c r="G15">
-        <f>HEX2DEC(RIGHT(D15,2))/2</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H15">
-        <f>HEX2DEC(LEFT(D15,2))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I15">
-        <f>G15*H15*2</f>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="J15" t="str">
-        <f>DEC2HEX(HEX2DEC(B15)+I15)</f>
-        <v>DB74</v>
+        <f t="shared" si="3"/>
+        <v>DBB0</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DB2C $3b15 $3b3e ; MST in shop</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DB68 $3b15 $3b3e ; MST in shop</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
@@ -2245,7 +2248,7 @@
       </c>
       <c r="B16" t="str">
         <f>J15</f>
-        <v>DB74</v>
+        <v>DBB0</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
@@ -2260,24 +2263,24 @@
         <v>124</v>
       </c>
       <c r="G16">
-        <f>HEX2DEC(RIGHT(D16,2))/2</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H16">
-        <f>HEX2DEC(LEFT(D16,2))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I16">
-        <f>G16*H16*2</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="J16" t="str">
-        <f>DEC2HEX(HEX2DEC(B16)+I16)</f>
-        <v>DBB0</v>
+        <f t="shared" si="3"/>
+        <v>DBEC</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DB74 $3895 $38b5 ; Buy/Sell</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DBB0 $3895 $38b5 ; Buy/Sell</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
@@ -2286,7 +2289,7 @@
       </c>
       <c r="B17" t="str">
         <f>J10</f>
-        <v>DB7C</v>
+        <v>DBB8</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>88</v>
@@ -2301,24 +2304,24 @@
         <v>118</v>
       </c>
       <c r="G17">
-        <f>HEX2DEC(RIGHT(D17,2))/2</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="H17">
-        <f>HEX2DEC(LEFT(D17,2))</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="I17">
-        <f>G17*H17*2</f>
+        <f t="shared" si="2"/>
         <v>364</v>
       </c>
       <c r="J17" t="str">
-        <f>DEC2HEX(HEX2DEC(B17)+I17)</f>
-        <v>DCE8</v>
+        <f t="shared" si="3"/>
+        <v>DD24</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DB7C $38fc $39df ; Character stats</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DBB8 $38fc $39df ; Character stats</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
@@ -2327,7 +2330,7 @@
       </c>
       <c r="B18" t="str">
         <f>B17</f>
-        <v>DB7C</v>
+        <v>DBB8</v>
       </c>
       <c r="C18" t="s">
         <v>50</v>
@@ -2342,24 +2345,24 @@
         <v>116</v>
       </c>
       <c r="G18">
-        <f>HEX2DEC(RIGHT(D18,2))/2</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H18">
-        <f>HEX2DEC(LEFT(D18,2))</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="I18">
-        <f>G18*H18*2</f>
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="J18" t="str">
-        <f>DEC2HEX(HEX2DEC(B18)+I18)</f>
-        <v>DBDE</v>
+        <f t="shared" si="3"/>
+        <v>DC1A</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DB7C $3877 $3889 ; Use, Equip, Drop</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DBB8 $3877 $3889 ; Use, Equip, Drop</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
@@ -2368,7 +2371,7 @@
       </c>
       <c r="B19" t="str">
         <f>J14</f>
-        <v>DBBC</v>
+        <v>DBF8</v>
       </c>
       <c r="C19" t="s">
         <v>30</v>
@@ -2383,24 +2386,24 @@
         <v>121</v>
       </c>
       <c r="G19">
-        <f>HEX2DEC(RIGHT(D19,2))/2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H19">
-        <f>HEX2DEC(LEFT(D19,2))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I19">
-        <f>G19*H19*2</f>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="J19" t="str">
-        <f>DEC2HEX(HEX2DEC(B19)+I19)</f>
-        <v>DBEC</v>
+        <f t="shared" si="3"/>
+        <v>DC28</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DBBC $3015 $3036 ; Active player (during battle)</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DBF8 $3015 $3036 ; Active player (during battle)</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
@@ -2409,7 +2412,7 @@
       </c>
       <c r="B20" t="str">
         <f>J19</f>
-        <v>DBEC</v>
+        <v>DC28</v>
       </c>
       <c r="C20" t="s">
         <v>43</v>
@@ -2424,24 +2427,24 @@
         <v>112</v>
       </c>
       <c r="G20">
-        <f>HEX2DEC(RIGHT(D20,2))/2</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H20">
-        <f>HEX2DEC(LEFT(D20,2))</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="I20">
-        <f>G20*H20*2</f>
+        <f t="shared" si="2"/>
         <v>504</v>
       </c>
       <c r="J20" t="str">
-        <f>DEC2HEX(HEX2DEC(B20)+I20)</f>
-        <v>DDE4</v>
+        <f t="shared" si="3"/>
+        <v>DE20</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DBEC $363c $3775 ; Inventory</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DC28 $363c $3775 ; Inventory</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
@@ -2450,7 +2453,7 @@
       </c>
       <c r="B21" t="str">
         <f>J17</f>
-        <v>DCE8</v>
+        <v>DD24</v>
       </c>
       <c r="C21" t="s">
         <v>41</v>
@@ -2465,24 +2468,24 @@
         <v>114</v>
       </c>
       <c r="G21">
-        <f>HEX2DEC(RIGHT(D21,2))/2</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H21">
-        <f>HEX2DEC(LEFT(D21,2))</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="I21">
-        <f>G21*H21*2</f>
+        <f t="shared" si="2"/>
         <v>288</v>
       </c>
       <c r="J21" t="str">
-        <f>DEC2HEX(HEX2DEC(B21)+I21)</f>
-        <v>DE08</v>
+        <f t="shared" si="3"/>
+        <v>DE44</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DCE8 $3595 $35e4 ; Spell list</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DD24 $3595 $35e4 ; Spell list</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
@@ -2491,7 +2494,7 @@
       </c>
       <c r="B22" t="str">
         <f>J21</f>
-        <v>DE08</v>
+        <v>DE44</v>
       </c>
       <c r="C22" t="s">
         <v>45</v>
@@ -2506,24 +2509,24 @@
         <v>113</v>
       </c>
       <c r="G22">
-        <f>HEX2DEC(RIGHT(D22,2))/2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H22">
-        <f>HEX2DEC(LEFT(D22,2))</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="I22">
-        <f>G22*H22*2</f>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="J22" t="str">
-        <f>DEC2HEX(HEX2DEC(B22)+I22)</f>
-        <v>DE98</v>
+        <f t="shared" si="3"/>
+        <v>DED4</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DE08 $3788 $37de ; Player select</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DE44 $3788 $37de ; Player select</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
@@ -2532,7 +2535,7 @@
       </c>
       <c r="B23" t="str">
         <f>B22</f>
-        <v>DE08</v>
+        <v>DE44</v>
       </c>
       <c r="C23" t="s">
         <v>54</v>
@@ -2547,24 +2550,24 @@
         <v>125</v>
       </c>
       <c r="G23">
-        <f>HEX2DEC(RIGHT(D23,2))/2</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H23">
-        <f>HEX2DEC(LEFT(D23,2))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I23">
-        <f>G23*H23*2</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="J23" t="str">
-        <f>DEC2HEX(HEX2DEC(B23)+I23)</f>
-        <v>DE3A</v>
+        <f t="shared" si="3"/>
+        <v>DE76</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DE08 $38c1 $38e1 ; Yes/No</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DE44 $38c1 $38e1 ; Yes/No</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">
@@ -2573,7 +2576,7 @@
       </c>
       <c r="B24" t="str">
         <f>J22</f>
-        <v>DE98</v>
+        <v>DED4</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
@@ -2588,24 +2591,24 @@
         <v>115</v>
       </c>
       <c r="G24">
-        <f>HEX2DEC(RIGHT(D24,2))/2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H24">
-        <f>HEX2DEC(LEFT(D24,2))</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="I24">
-        <f>G24*H24*2</f>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="J24" t="str">
-        <f>DEC2HEX(HEX2DEC(B24)+I24)</f>
-        <v>DF28</v>
+        <f t="shared" si="3"/>
+        <v>DF64</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DE98 $37a5 $37ef ; Player select for magic</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">  PatchWindow $DED4 $37a5 $37ef ; Player select for magic</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Widened item names to 11
</commit_message>
<xml_diff>
--- a/psrp/RAM windows cache.xlsx
+++ b/psrp/RAM windows cache.xlsx
@@ -421,9 +421,6 @@
     <t>0b10</t>
   </si>
   <si>
-    <t>0418</t>
-  </si>
-  <si>
     <t>0310</t>
   </si>
   <si>
@@ -439,15 +436,6 @@
     <t>0e1a</t>
   </si>
   <si>
-    <t>0818</t>
-  </si>
-  <si>
-    <t>1518</t>
-  </si>
-  <si>
-    <t>0318</t>
-  </si>
-  <si>
     <t>0824</t>
   </si>
   <si>
@@ -467,6 +455,18 @@
   </si>
   <si>
     <t>0330</t>
+  </si>
+  <si>
+    <t>081a</t>
+  </si>
+  <si>
+    <t>151a</t>
+  </si>
+  <si>
+    <t>0319</t>
+  </si>
+  <si>
+    <t>041a</t>
   </si>
 </sst>
 </file>
@@ -1661,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1803,7 +1803,7 @@
         <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -1844,13 +1844,13 @@
         <v>39</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E6" t="s">
         <v>105</v>
       </c>
       <c r="F6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -1891,7 +1891,7 @@
         <v>96</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -1967,7 +1967,7 @@
         <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -2008,7 +2008,7 @@
         <v>49</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
@@ -2018,7 +2018,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
@@ -2026,11 +2026,11 @@
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="3"/>
-        <v>DBB8</v>
+        <v>DBC8</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="4"/>
@@ -2090,7 +2090,7 @@
         <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="E12" t="s">
         <v>94</v>
@@ -2100,7 +2100,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
@@ -2108,11 +2108,11 @@
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="3"/>
-        <v>DB58</v>
+        <v>DB60</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="4"/>
@@ -2131,7 +2131,7 @@
         <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E13" t="s">
         <v>103</v>
@@ -2166,7 +2166,7 @@
       </c>
       <c r="B14" t="str">
         <f>J12</f>
-        <v>DB58</v>
+        <v>DB60</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>83</v>
@@ -2175,7 +2175,7 @@
         <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F14" t="s">
         <v>120</v>
@@ -2194,11 +2194,11 @@
       </c>
       <c r="J14" t="str">
         <f t="shared" si="3"/>
-        <v>DBF8</v>
+        <v>DC00</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DB58 $3262 $330a ; Enemy stats (up to 8)</v>
+        <v xml:space="preserve">  PatchWindow $DB60 $3262 $330a ; Enemy stats (up to 8)</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
@@ -2213,7 +2213,7 @@
         <v>91</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E15" t="s">
         <v>98</v>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
@@ -2231,11 +2231,11 @@
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="3"/>
-        <v>DBB0</v>
+        <v>DBB3</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="4"/>
@@ -2248,7 +2248,7 @@
       </c>
       <c r="B16" t="str">
         <f>J15</f>
-        <v>DBB0</v>
+        <v>DBB3</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
@@ -2276,11 +2276,11 @@
       </c>
       <c r="J16" t="str">
         <f t="shared" si="3"/>
-        <v>DBEC</v>
+        <v>DBEF</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DBB0 $3895 $38b5 ; Buy/Sell</v>
+        <v xml:space="preserve">  PatchWindow $DBB3 $3895 $38b5 ; Buy/Sell</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
@@ -2289,13 +2289,13 @@
       </c>
       <c r="B17" t="str">
         <f>J10</f>
-        <v>DBB8</v>
+        <v>DBC8</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -2317,11 +2317,11 @@
       </c>
       <c r="J17" t="str">
         <f t="shared" si="3"/>
-        <v>DD24</v>
+        <v>DD34</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DBB8 $38fc $39df ; Character stats</v>
+        <v xml:space="preserve">  PatchWindow $DBC8 $38fc $39df ; Character stats</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
@@ -2330,13 +2330,13 @@
       </c>
       <c r="B18" t="str">
         <f>B17</f>
-        <v>DBB8</v>
+        <v>DBC8</v>
       </c>
       <c r="C18" t="s">
         <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E18" t="s">
         <v>18</v>
@@ -2358,11 +2358,11 @@
       </c>
       <c r="J18" t="str">
         <f t="shared" si="3"/>
-        <v>DC1A</v>
+        <v>DC2A</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DBB8 $3877 $3889 ; Use, Equip, Drop</v>
+        <v xml:space="preserve">  PatchWindow $DBC8 $3877 $3889 ; Use, Equip, Drop</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
@@ -2371,13 +2371,13 @@
       </c>
       <c r="B19" t="str">
         <f>J14</f>
-        <v>DBF8</v>
+        <v>DC00</v>
       </c>
       <c r="C19" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E19" t="s">
         <v>22</v>
@@ -2399,11 +2399,11 @@
       </c>
       <c r="J19" t="str">
         <f t="shared" si="3"/>
-        <v>DC28</v>
+        <v>DC30</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DBF8 $3015 $3036 ; Active player (during battle)</v>
+        <v xml:space="preserve">  PatchWindow $DC00 $3015 $3036 ; Active player (during battle)</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
@@ -2412,13 +2412,13 @@
       </c>
       <c r="B20" t="str">
         <f>J19</f>
-        <v>DC28</v>
+        <v>DC30</v>
       </c>
       <c r="C20" t="s">
         <v>43</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E20" t="s">
         <v>69</v>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
@@ -2436,15 +2436,15 @@
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>504</v>
+        <v>546</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="3"/>
-        <v>DE20</v>
+        <v>DE52</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DC28 $363c $3775 ; Inventory</v>
+        <v xml:space="preserve">  PatchWindow $DC30 $363c $3775 ; Inventory</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
@@ -2453,13 +2453,13 @@
       </c>
       <c r="B21" t="str">
         <f>J17</f>
-        <v>DD24</v>
+        <v>DD34</v>
       </c>
       <c r="C21" t="s">
         <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -2481,11 +2481,11 @@
       </c>
       <c r="J21" t="str">
         <f t="shared" si="3"/>
-        <v>DE44</v>
+        <v>DE54</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DD24 $3595 $35e4 ; Spell list</v>
+        <v xml:space="preserve">  PatchWindow $DD34 $3595 $35e4 ; Spell list</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
@@ -2494,13 +2494,13 @@
       </c>
       <c r="B22" t="str">
         <f>J21</f>
-        <v>DE44</v>
+        <v>DE54</v>
       </c>
       <c r="C22" t="s">
         <v>45</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
@@ -2522,11 +2522,11 @@
       </c>
       <c r="J22" t="str">
         <f t="shared" si="3"/>
-        <v>DED4</v>
+        <v>DEE4</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DE44 $3788 $37de ; Player select</v>
+        <v xml:space="preserve">  PatchWindow $DE54 $3788 $37de ; Player select</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
@@ -2535,7 +2535,7 @@
       </c>
       <c r="B23" t="str">
         <f>B22</f>
-        <v>DE44</v>
+        <v>DE54</v>
       </c>
       <c r="C23" t="s">
         <v>54</v>
@@ -2563,11 +2563,11 @@
       </c>
       <c r="J23" t="str">
         <f t="shared" si="3"/>
-        <v>DE76</v>
+        <v>DE86</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DE44 $38c1 $38e1 ; Yes/No</v>
+        <v xml:space="preserve">  PatchWindow $DE54 $38c1 $38e1 ; Yes/No</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">
@@ -2576,13 +2576,13 @@
       </c>
       <c r="B24" t="str">
         <f>J22</f>
-        <v>DED4</v>
+        <v>DEE4</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E24" t="s">
         <v>17</v>
@@ -2604,11 +2604,11 @@
       </c>
       <c r="J24" t="str">
         <f t="shared" si="3"/>
-        <v>DF64</v>
+        <v>DF74</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DED4 $37a5 $37ef ; Player select for magic</v>
+        <v xml:space="preserve">  PatchWindow $DEE4 $37a5 $37ef ; Player select for magic</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Increase item names width to 14 chars - almost no wrapping now
</commit_message>
<xml_diff>
--- a/psrp/RAM windows cache.xlsx
+++ b/psrp/RAM windows cache.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$J$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$2:$J$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">Sheet2!$A$2:$J$24</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="145">
   <si>
     <t>What</t>
   </si>
@@ -433,12 +433,6 @@
     <t>0c18</t>
   </si>
   <si>
-    <t>0e1a</t>
-  </si>
-  <si>
-    <t>0824</t>
-  </si>
-  <si>
     <t>080e</t>
   </si>
   <si>
@@ -457,16 +451,19 @@
     <t>0330</t>
   </si>
   <si>
-    <t>081a</t>
-  </si>
-  <si>
-    <t>151a</t>
-  </si>
-  <si>
-    <t>0319</t>
-  </si>
-  <si>
-    <t>041a</t>
+    <t>082c</t>
+  </si>
+  <si>
+    <t>0420</t>
+  </si>
+  <si>
+    <t>0e20</t>
+  </si>
+  <si>
+    <t>1520</t>
+  </si>
+  <si>
+    <t>031a</t>
   </si>
 </sst>
 </file>
@@ -1661,23 +1658,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="3" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.73046875" customWidth="1"/>
+    <col min="2" max="2" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.9296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1689,28 +1687,28 @@
         <v>65</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>106</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
@@ -1720,36 +1718,36 @@
       <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="str">
+        <f>DEC2HEX(HEX2DEC(B3)+J3)</f>
+        <v>D880</v>
+      </c>
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>108</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G24" si="0">HEX2DEC(RIGHT(D3,2))/2</f>
+      <c r="H3">
+        <f>HEX2DEC(RIGHT(E3,2))/2</f>
         <v>32</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H24" si="1">HEX2DEC(LEFT(D3,2))</f>
+      <c r="I3">
+        <f>HEX2DEC(LEFT(E3,2))</f>
         <v>6</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I24" si="2">G3*H3*2</f>
+      <c r="J3">
+        <f>H3*I3*2</f>
         <v>384</v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J24" si="3">DEC2HEX(HEX2DEC(B3)+I3)</f>
-        <v>D880</v>
-      </c>
       <c r="K3" t="str">
-        <f>"  PatchWindow $"&amp;B3&amp;" $"&amp;LOWER(DEC2HEX(HEX2DEC(A3)+1))&amp;" $"&amp;LOWER(DEC2HEX(HEX2DEC(F3)+1))&amp;" ; "&amp;E3</f>
+        <f>"  PatchWindow $"&amp;B3&amp;" $"&amp;LOWER(DEC2HEX(HEX2DEC(A3)+1))&amp;" $"&amp;LOWER(DEC2HEX(HEX2DEC(G3)+1))&amp;" ; "&amp;F3</f>
         <v xml:space="preserve">  PatchWindow $d700 $3042 $3220 ; Party stats</v>
       </c>
     </row>
@@ -1761,33 +1759,33 @@
         <f>B3</f>
         <v>d700</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="str">
+        <f>DEC2HEX(HEX2DEC(B4)+J4)</f>
+        <v>D880</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>100</v>
       </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
+      <c r="H4">
+        <f>HEX2DEC(RIGHT(E4,2))/2</f>
         <v>32</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
+      <c r="I4">
+        <f>HEX2DEC(LEFT(E4,2))</f>
         <v>6</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="2"/>
+      <c r="J4">
+        <f>H4*I4*2</f>
         <v>384</v>
       </c>
-      <c r="J4" t="str">
-        <f t="shared" si="3"/>
-        <v>D880</v>
-      </c>
       <c r="K4" t="str">
-        <f t="shared" ref="K4:K24" si="4">"  PatchWindow $"&amp;B4&amp;" $"&amp;LOWER(DEC2HEX(HEX2DEC(A4)+1))&amp;" $"&amp;LOWER(DEC2HEX(HEX2DEC(F4)+1))&amp;" ; "&amp;E4</f>
+        <f t="shared" ref="K4:K24" si="0">"  PatchWindow $"&amp;B4&amp;" $"&amp;LOWER(DEC2HEX(HEX2DEC(A4)+1))&amp;" $"&amp;LOWER(DEC2HEX(HEX2DEC(G4)+1))&amp;" ; "&amp;F4</f>
         <v xml:space="preserve">  PatchWindow $d700 $30fd $1 ; Party stats again</v>
       </c>
     </row>
@@ -1796,39 +1794,39 @@
         <v>68</v>
       </c>
       <c r="B5" t="str">
-        <f>J3</f>
+        <f>C3</f>
         <v>D880</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="str">
+        <f>DEC2HEX(HEX2DEC(B5)+J5)</f>
+        <v>D9B8</v>
+      </c>
+      <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>110</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
+      <c r="H5">
+        <f>HEX2DEC(RIGHT(E5,2))/2</f>
         <v>26</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
+      <c r="I5">
+        <f>HEX2DEC(LEFT(E5,2))</f>
         <v>6</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="2"/>
+      <c r="J5">
+        <f>H5*I5*2</f>
         <v>312</v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" si="3"/>
-        <v>D9B8</v>
-      </c>
       <c r="K5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">  PatchWindow $D880 $334d $3587 ; Narrative box</v>
       </c>
     </row>
@@ -1837,39 +1835,39 @@
         <v>84</v>
       </c>
       <c r="B6" t="str">
-        <f>J5</f>
+        <f>C5</f>
         <v>D9B8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="str">
+        <f>DEC2HEX(HEX2DEC(B6)+J6)</f>
+        <v>DA48</v>
+      </c>
+      <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" t="s">
         <v>105</v>
       </c>
-      <c r="F6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
+      <c r="G6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6">
+        <f>HEX2DEC(RIGHT(E6,2))/2</f>
         <v>24</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
+      <c r="I6">
+        <f>HEX2DEC(LEFT(E6,2))</f>
         <v>3</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="2"/>
+      <c r="J6">
+        <f>H6*I6*2</f>
         <v>144</v>
       </c>
-      <c r="J6" t="str">
-        <f t="shared" si="3"/>
-        <v>DA48</v>
-      </c>
       <c r="K6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">  PatchWindow $D9B8 $3554 $3560 ; Narrative box scroll buffer</v>
       </c>
     </row>
@@ -1878,39 +1876,39 @@
         <v>79</v>
       </c>
       <c r="B7" t="str">
-        <f>J6</f>
+        <f>C6</f>
         <v>DA48</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="str">
+        <f>DEC2HEX(HEX2DEC(B7)+J7)</f>
+        <v>DAF8</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>129</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
+      <c r="G7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7">
+        <f>HEX2DEC(RIGHT(E7,2))/2</f>
         <v>8</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
+      <c r="I7">
+        <f>HEX2DEC(LEFT(E7,2))</f>
         <v>11</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="2"/>
+      <c r="J7">
+        <f>H7*I7*2</f>
         <v>176</v>
       </c>
-      <c r="J7" t="str">
-        <f t="shared" si="3"/>
-        <v>DAF8</v>
-      </c>
       <c r="K7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">  PatchWindow $DA48 $322c $324a ; Battle menu</v>
       </c>
     </row>
@@ -1922,36 +1920,36 @@
         <f>B7</f>
         <v>DA48</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="str">
+        <f>DEC2HEX(HEX2DEC(B8)+J8)</f>
+        <v>DAF8</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>129</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>93</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>107</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
+      <c r="H8">
+        <f>HEX2DEC(RIGHT(E8,2))/2</f>
         <v>8</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
+      <c r="I8">
+        <f>HEX2DEC(LEFT(E8,2))</f>
         <v>11</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="2"/>
+      <c r="J8">
+        <f>H8*I8*2</f>
         <v>176</v>
       </c>
-      <c r="J8" t="str">
-        <f t="shared" si="3"/>
-        <v>DAF8</v>
-      </c>
       <c r="K8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">  PatchWindow $DA48 $37fb $3819 ; Regular world menu</v>
       </c>
     </row>
@@ -1963,36 +1961,36 @@
         <f>B8</f>
         <v>DA48</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="str">
+        <f>DEC2HEX(HEX2DEC(B9)+J9)</f>
+        <v>DBA8</v>
+      </c>
+      <c r="D9" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>126</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f>HEX2DEC(RIGHT(E9,2))/2</f>
+        <v>22</v>
+      </c>
+      <c r="I9">
+        <f>HEX2DEC(LEFT(E9,2))</f>
         <v>8</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="2"/>
-        <v>288</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="3"/>
-        <v>DB68</v>
+      <c r="J9">
+        <f>H9*I9*2</f>
+        <v>352</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">  PatchWindow $DA48 $39eb $3ac4 ; Shop items</v>
       </c>
     </row>
@@ -2001,39 +1999,39 @@
         <v>75</v>
       </c>
       <c r="B10" t="str">
-        <f>J8</f>
+        <f>C8</f>
         <v>DAF8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="str">
+        <f>DEC2HEX(HEX2DEC(B10)+J10)</f>
+        <v>DBF8</v>
+      </c>
+      <c r="D10" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s">
         <v>20</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>117</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f>HEX2DEC(RIGHT(E10,2))/2</f>
+        <v>16</v>
+      </c>
+      <c r="I10">
+        <f>HEX2DEC(LEFT(E10,2))</f>
         <v>8</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="2"/>
-        <v>208</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="3"/>
-        <v>DBC8</v>
+      <c r="J10">
+        <f>H10*I10*2</f>
+        <v>256</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">  PatchWindow $DAF8 $3826 $386b ; Currently equipped items</v>
       </c>
     </row>
@@ -2045,36 +2043,36 @@
         <f>B10</f>
         <v>DAF8</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="str">
+        <f>DEC2HEX(HEX2DEC(B11)+J11)</f>
+        <v>DBD0</v>
+      </c>
+      <c r="D11" t="s">
         <v>59</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>60</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>99</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>122</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
+      <c r="H11">
+        <f>HEX2DEC(RIGHT(E11,2))/2</f>
         <v>9</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
+      <c r="I11">
+        <f>HEX2DEC(LEFT(E11,2))</f>
         <v>12</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="2"/>
+      <c r="J11">
+        <f>H11*I11*2</f>
         <v>216</v>
       </c>
-      <c r="J11" t="str">
-        <f t="shared" si="3"/>
-        <v>DBD0</v>
-      </c>
       <c r="K11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">  PatchWindow $DAF8 $3ad0 $3b08 ; Select save slot</v>
       </c>
     </row>
@@ -2086,36 +2084,36 @@
         <f>B11</f>
         <v>DAF8</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="str">
+        <f>DEC2HEX(HEX2DEC(B12)+J12)</f>
+        <v>DB78</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" t="s">
         <v>94</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>119</v>
       </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f>HEX2DEC(RIGHT(E12,2))/2</f>
+        <v>16</v>
+      </c>
+      <c r="I12">
+        <f>HEX2DEC(LEFT(E12,2))</f>
         <v>4</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="2"/>
-        <v>104</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="3"/>
-        <v>DB60</v>
+      <c r="J12">
+        <f>H12*I12*2</f>
+        <v>128</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">  PatchWindow $DAF8 $3256 $331b ; Enemy name</v>
       </c>
     </row>
@@ -2124,40 +2122,40 @@
         <v>92</v>
       </c>
       <c r="B13" t="str">
-        <f>B12</f>
-        <v>DAF8</v>
-      </c>
-      <c r="C13" t="s">
+        <f>C18</f>
+        <v>DB5A</v>
+      </c>
+      <c r="C13" t="str">
+        <f>DEC2HEX(HEX2DEC(B13)+J13)</f>
+        <v>DBCA</v>
+      </c>
+      <c r="D13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" t="s">
-        <v>136</v>
-      </c>
       <c r="E13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" t="s">
         <v>103</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>128</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
+      <c r="H13">
+        <f>HEX2DEC(RIGHT(E13,2))/2</f>
         <v>7</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
+      <c r="I13">
+        <f>HEX2DEC(LEFT(E13,2))</f>
         <v>8</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="2"/>
+      <c r="J13">
+        <f>H13*I13*2</f>
         <v>112</v>
       </c>
-      <c r="J13" t="str">
-        <f t="shared" si="3"/>
-        <v>DB68</v>
-      </c>
       <c r="K13" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DAF8 $3b4c $3b73 ; Hapsby travel</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  PatchWindow $DB5A $3b4c $3b73 ; Hapsby travel</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
@@ -2165,40 +2163,40 @@
         <v>82</v>
       </c>
       <c r="B14" t="str">
-        <f>J12</f>
-        <v>DB60</v>
-      </c>
-      <c r="C14" s="1" t="s">
+        <f>C12</f>
+        <v>DB78</v>
+      </c>
+      <c r="C14" t="str">
+        <f>DEC2HEX(HEX2DEC(B14)+J14)</f>
+        <v>DC18</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E14" t="s">
-        <v>139</v>
-      </c>
       <c r="F14" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" t="s">
         <v>120</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
+      <c r="H14">
+        <f>HEX2DEC(RIGHT(E14,2))/2</f>
         <v>8</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
+      <c r="I14">
+        <f>HEX2DEC(LEFT(E14,2))</f>
         <v>10</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="2"/>
+      <c r="J14">
+        <f>H14*I14*2</f>
         <v>160</v>
       </c>
-      <c r="J14" t="str">
-        <f t="shared" si="3"/>
-        <v>DC00</v>
-      </c>
       <c r="K14" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DB60 $3262 $330a ; Enemy stats (up to 8)</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  PatchWindow $DB78 $3262 $330a ; Enemy stats (up to 8)</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
@@ -2206,40 +2204,40 @@
         <v>77</v>
       </c>
       <c r="B15" t="str">
-        <f>J9</f>
-        <v>DB68</v>
-      </c>
-      <c r="C15" t="s">
+        <f>C9</f>
+        <v>DBA8</v>
+      </c>
+      <c r="C15" t="str">
+        <f>DEC2HEX(HEX2DEC(B15)+J15)</f>
+        <v>DBF6</v>
+      </c>
+      <c r="D15" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>98</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>127</v>
       </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>12.5</v>
-      </c>
       <c r="H15">
-        <f t="shared" si="1"/>
+        <f>HEX2DEC(RIGHT(E15,2))/2</f>
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <f>HEX2DEC(LEFT(E15,2))</f>
         <v>3</v>
       </c>
-      <c r="I15">
-        <f t="shared" si="2"/>
-        <v>75</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="3"/>
-        <v>DBB3</v>
+      <c r="J15">
+        <f>H15*I15*2</f>
+        <v>78</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DB68 $3b15 $3b3e ; MST in shop</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  PatchWindow $DBA8 $3b15 $3b3e ; MST in shop</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
@@ -2247,40 +2245,40 @@
         <v>85</v>
       </c>
       <c r="B16" t="str">
-        <f>J15</f>
-        <v>DBB3</v>
-      </c>
-      <c r="C16" t="s">
+        <f>C10</f>
+        <v>DBF8</v>
+      </c>
+      <c r="C16" t="str">
+        <f>DEC2HEX(HEX2DEC(B16)+J16)</f>
+        <v>DC34</v>
+      </c>
+      <c r="D16" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>104</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>124</v>
       </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
+      <c r="H16">
+        <f>HEX2DEC(RIGHT(E16,2))/2</f>
         <v>6</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
+      <c r="I16">
+        <f>HEX2DEC(LEFT(E16,2))</f>
         <v>5</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="2"/>
+      <c r="J16">
+        <f>H16*I16*2</f>
         <v>60</v>
       </c>
-      <c r="J16" t="str">
-        <f t="shared" si="3"/>
-        <v>DBEF</v>
-      </c>
       <c r="K16" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DBB3 $3895 $38b5 ; Buy/Sell</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  PatchWindow $DBF8 $3895 $38b5 ; Buy/Sell</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
@@ -2288,40 +2286,40 @@
         <v>87</v>
       </c>
       <c r="B17" t="str">
-        <f>J10</f>
-        <v>DBC8</v>
-      </c>
-      <c r="C17" s="1" t="s">
+        <f>B5</f>
+        <v>D880</v>
+      </c>
+      <c r="C17" t="str">
+        <f>DEC2HEX(HEX2DEC(B17)+J17)</f>
+        <v>DA40</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F17" t="s">
         <v>6</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>118</v>
       </c>
-      <c r="G17">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
       <c r="H17">
-        <f t="shared" si="1"/>
+        <f>HEX2DEC(RIGHT(E17,2))/2</f>
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <f>HEX2DEC(LEFT(E17,2))</f>
         <v>14</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="2"/>
-        <v>364</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="3"/>
-        <v>DD34</v>
+      <c r="J17">
+        <f>H17*I17*2</f>
+        <v>448</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DBC8 $38fc $39df ; Character stats</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  PatchWindow $D880 $38fc $39df ; Character stats</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
@@ -2329,40 +2327,40 @@
         <v>74</v>
       </c>
       <c r="B18" t="str">
-        <f>B17</f>
-        <v>DBC8</v>
-      </c>
-      <c r="C18" t="s">
+        <f>C8</f>
+        <v>DAF8</v>
+      </c>
+      <c r="C18" t="str">
+        <f>DEC2HEX(HEX2DEC(B18)+J18)</f>
+        <v>DB5A</v>
+      </c>
+      <c r="D18" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>132</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>18</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>116</v>
       </c>
-      <c r="G18">
-        <f t="shared" si="0"/>
+      <c r="H18">
+        <f>HEX2DEC(RIGHT(E18,2))/2</f>
         <v>7</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="1"/>
+      <c r="I18">
+        <f>HEX2DEC(LEFT(E18,2))</f>
         <v>7</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="2"/>
+      <c r="J18">
+        <f>H18*I18*2</f>
         <v>98</v>
       </c>
-      <c r="J18" t="str">
-        <f t="shared" si="3"/>
-        <v>DC2A</v>
-      </c>
       <c r="K18" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DBC8 $3877 $3889 ; Use, Equip, Drop</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  PatchWindow $DAF8 $3877 $3889 ; Use, Equip, Drop</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
@@ -2370,40 +2368,40 @@
         <v>76</v>
       </c>
       <c r="B19" t="str">
-        <f>J14</f>
-        <v>DC00</v>
-      </c>
-      <c r="C19" t="s">
+        <f>C14</f>
+        <v>DC18</v>
+      </c>
+      <c r="C19" t="str">
+        <f>DEC2HEX(HEX2DEC(B19)+J19)</f>
+        <v>DC48</v>
+      </c>
+      <c r="D19" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>22</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>121</v>
       </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
+      <c r="H19">
+        <f>HEX2DEC(RIGHT(E19,2))/2</f>
         <v>8</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="1"/>
+      <c r="I19">
+        <f>HEX2DEC(LEFT(E19,2))</f>
         <v>3</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="2"/>
+      <c r="J19">
+        <f>H19*I19*2</f>
         <v>48</v>
       </c>
-      <c r="J19" t="str">
-        <f t="shared" si="3"/>
-        <v>DC30</v>
-      </c>
       <c r="K19" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DC00 $3015 $3036 ; Active player (during battle)</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  PatchWindow $DC18 $3015 $3036 ; Active player (during battle)</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
@@ -2411,40 +2409,40 @@
         <v>70</v>
       </c>
       <c r="B20" t="str">
-        <f>J19</f>
-        <v>DC30</v>
-      </c>
-      <c r="C20" t="s">
+        <f>C22</f>
+        <v>DC88</v>
+      </c>
+      <c r="C20" t="str">
+        <f>DEC2HEX(HEX2DEC(B20)+J20)</f>
+        <v>DF28</v>
+      </c>
+      <c r="D20" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>69</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>112</v>
       </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
       <c r="H20">
-        <f t="shared" si="1"/>
+        <f>HEX2DEC(RIGHT(E20,2))/2</f>
+        <v>16</v>
+      </c>
+      <c r="I20">
+        <f>HEX2DEC(LEFT(E20,2))</f>
         <v>21</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="2"/>
-        <v>546</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="3"/>
-        <v>DE52</v>
+      <c r="J20">
+        <f>H20*I20*2</f>
+        <v>672</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DC30 $363c $3775 ; Inventory</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  PatchWindow $DC88 $363c $3775 ; Inventory</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
@@ -2452,40 +2450,40 @@
         <v>72</v>
       </c>
       <c r="B21" t="str">
-        <f>J17</f>
-        <v>DD34</v>
-      </c>
-      <c r="C21" t="s">
+        <f>C22</f>
+        <v>DC88</v>
+      </c>
+      <c r="C21" t="str">
+        <f>DEC2HEX(HEX2DEC(B21)+J21)</f>
+        <v>DDA8</v>
+      </c>
+      <c r="D21" t="s">
         <v>41</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>133</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>12</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>114</v>
       </c>
-      <c r="G21">
-        <f t="shared" si="0"/>
+      <c r="H21">
+        <f>HEX2DEC(RIGHT(E21,2))/2</f>
         <v>12</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="1"/>
+      <c r="I21">
+        <f>HEX2DEC(LEFT(E21,2))</f>
         <v>12</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="2"/>
+      <c r="J21">
+        <f>H21*I21*2</f>
         <v>288</v>
       </c>
-      <c r="J21" t="str">
-        <f t="shared" si="3"/>
-        <v>DE54</v>
-      </c>
       <c r="K21" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DD34 $3595 $35e4 ; Spell list</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  PatchWindow $DC88 $3595 $35e4 ; Spell list</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
@@ -2493,40 +2491,40 @@
         <v>71</v>
       </c>
       <c r="B22" t="str">
-        <f>J21</f>
-        <v>DE54</v>
-      </c>
-      <c r="C22" t="s">
+        <f>C10</f>
+        <v>DBF8</v>
+      </c>
+      <c r="C22" t="str">
+        <f>DEC2HEX(HEX2DEC(B22)+J22)</f>
+        <v>DC88</v>
+      </c>
+      <c r="D22" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>15</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>113</v>
       </c>
-      <c r="G22">
-        <f t="shared" si="0"/>
+      <c r="H22">
+        <f>HEX2DEC(RIGHT(E22,2))/2</f>
         <v>8</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="1"/>
+      <c r="I22">
+        <f>HEX2DEC(LEFT(E22,2))</f>
         <v>9</v>
       </c>
-      <c r="I22">
-        <f t="shared" si="2"/>
+      <c r="J22">
+        <f>H22*I22*2</f>
         <v>144</v>
       </c>
-      <c r="J22" t="str">
-        <f t="shared" si="3"/>
-        <v>DEE4</v>
-      </c>
       <c r="K22" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DE54 $3788 $37de ; Player select</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  PatchWindow $DBF8 $3788 $37de ; Player select</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
@@ -2534,40 +2532,40 @@
         <v>86</v>
       </c>
       <c r="B23" t="str">
-        <f>B22</f>
-        <v>DE54</v>
-      </c>
-      <c r="C23" t="s">
+        <f>C10</f>
+        <v>DBF8</v>
+      </c>
+      <c r="C23" t="str">
+        <f>DEC2HEX(HEX2DEC(B23)+J23)</f>
+        <v>DC2A</v>
+      </c>
+      <c r="D23" t="s">
         <v>54</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>55</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>97</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>125</v>
       </c>
-      <c r="G23">
-        <f t="shared" si="0"/>
+      <c r="H23">
+        <f>HEX2DEC(RIGHT(E23,2))/2</f>
         <v>5</v>
       </c>
-      <c r="H23">
-        <f t="shared" si="1"/>
+      <c r="I23">
+        <f>HEX2DEC(LEFT(E23,2))</f>
         <v>5</v>
       </c>
-      <c r="I23">
-        <f t="shared" si="2"/>
+      <c r="J23">
+        <f>H23*I23*2</f>
         <v>50</v>
       </c>
-      <c r="J23" t="str">
-        <f t="shared" si="3"/>
-        <v>DE86</v>
-      </c>
       <c r="K23" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DE54 $38c1 $38e1 ; Yes/No</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  PatchWindow $DBF8 $38c1 $38e1 ; Yes/No</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">
@@ -2575,40 +2573,40 @@
         <v>73</v>
       </c>
       <c r="B24" t="str">
-        <f>J22</f>
-        <v>DEE4</v>
-      </c>
-      <c r="C24" t="s">
+        <f>C21</f>
+        <v>DDA8</v>
+      </c>
+      <c r="C24" t="str">
+        <f>DEC2HEX(HEX2DEC(B24)+J24)</f>
+        <v>DE38</v>
+      </c>
+      <c r="D24" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>17</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>115</v>
       </c>
-      <c r="G24">
-        <f t="shared" si="0"/>
+      <c r="H24">
+        <f>HEX2DEC(RIGHT(E24,2))/2</f>
         <v>8</v>
       </c>
-      <c r="H24">
-        <f t="shared" si="1"/>
+      <c r="I24">
+        <f>HEX2DEC(LEFT(E24,2))</f>
         <v>9</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="2"/>
+      <c r="J24">
+        <f>H24*I24*2</f>
         <v>144</v>
       </c>
-      <c r="J24" t="str">
-        <f t="shared" si="3"/>
-        <v>DF74</v>
-      </c>
       <c r="K24" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">  PatchWindow $DEE4 $37a5 $37ef ; Player select for magic</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  PatchWindow $DDA8 $37a5 $37ef ; Player select for magic</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Show "Meseta" instead of "MST"
</commit_message>
<xml_diff>
--- a/psrp/RAM windows cache.xlsx
+++ b/psrp/RAM windows cache.xlsx
@@ -457,13 +457,13 @@
     <t>0420</t>
   </si>
   <si>
-    <t>0e20</t>
-  </si>
-  <si>
     <t>1520</t>
   </si>
   <si>
     <t>031a</t>
+  </si>
+  <si>
+    <t>0e1c</t>
   </si>
 </sst>
 </file>
@@ -1659,7 +1659,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2122,12 +2122,12 @@
         <v>92</v>
       </c>
       <c r="B13" t="str">
-        <f>C18</f>
-        <v>DB5A</v>
+        <f>B12</f>
+        <v>DAF8</v>
       </c>
       <c r="C13" t="str">
         <f>DEC2HEX(HEX2DEC(B13)+J13)</f>
-        <v>DBCA</v>
+        <v>DB68</v>
       </c>
       <c r="D13" t="s">
         <v>62</v>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DB5A $3b4c $3b73 ; Hapsby travel</v>
+        <v xml:space="preserve">  PatchWindow $DAF8 $3b4c $3b73 ; Hapsby travel</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
@@ -2215,7 +2215,7 @@
         <v>91</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F15" t="s">
         <v>98</v>
@@ -2291,13 +2291,13 @@
       </c>
       <c r="C17" t="str">
         <f>DEC2HEX(HEX2DEC(B17)+J17)</f>
-        <v>DA40</v>
+        <v>DA08</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>88</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="H17">
         <f>HEX2DEC(RIGHT(E17,2))/2</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I17">
         <f>HEX2DEC(LEFT(E17,2))</f>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="J17">
         <f>H17*I17*2</f>
-        <v>448</v>
+        <v>392</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
@@ -2327,12 +2327,12 @@
         <v>74</v>
       </c>
       <c r="B18" t="str">
-        <f>C8</f>
-        <v>DAF8</v>
+        <f>C20</f>
+        <v>DF28</v>
       </c>
       <c r="C18" t="str">
         <f>DEC2HEX(HEX2DEC(B18)+J18)</f>
-        <v>DB5A</v>
+        <v>DF8A</v>
       </c>
       <c r="D18" t="s">
         <v>50</v>
@@ -2360,7 +2360,7 @@
       </c>
       <c r="K18" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DAF8 $3877 $3889 ; Use, Equip, Drop</v>
+        <v xml:space="preserve">  PatchWindow $DF28 $3877 $3889 ; Use, Equip, Drop</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
@@ -2420,7 +2420,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F20" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Fixed screen corruption in hospitals (MST collided with player select)
</commit_message>
<xml_diff>
--- a/psrp/RAM windows cache.xlsx
+++ b/psrp/RAM windows cache.xlsx
@@ -454,16 +454,16 @@
     <t>082c</t>
   </si>
   <si>
-    <t>0420</t>
-  </si>
-  <si>
     <t>1520</t>
   </si>
   <si>
-    <t>031a</t>
-  </si>
-  <si>
     <t>0e1c</t>
+  </si>
+  <si>
+    <t>0320</t>
+  </si>
+  <si>
+    <t>032a</t>
   </si>
 </sst>
 </file>
@@ -1658,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2086,13 +2086,13 @@
       </c>
       <c r="C12" t="str">
         <f>DEC2HEX(HEX2DEC(B12)+J12)</f>
-        <v>DB78</v>
+        <v>DB76</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F12" t="s">
         <v>94</v>
@@ -2102,15 +2102,15 @@
       </c>
       <c r="H12">
         <f>HEX2DEC(RIGHT(E12,2))/2</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I12">
         <f>HEX2DEC(LEFT(E12,2))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12">
         <f>H12*I12*2</f>
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
@@ -2164,11 +2164,11 @@
       </c>
       <c r="B14" t="str">
         <f>C12</f>
-        <v>DB78</v>
+        <v>DB76</v>
       </c>
       <c r="C14" t="str">
         <f>DEC2HEX(HEX2DEC(B14)+J14)</f>
-        <v>DC18</v>
+        <v>DC16</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>83</v>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DB78 $3262 $330a ; Enemy stats (up to 8)</v>
+        <v xml:space="preserve">  PatchWindow $DB76 $3262 $330a ; Enemy stats (up to 8)</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
@@ -2204,12 +2204,12 @@
         <v>77</v>
       </c>
       <c r="B15" t="str">
-        <f>C9</f>
-        <v>DBA8</v>
+        <f>C22</f>
+        <v>DC88</v>
       </c>
       <c r="C15" t="str">
         <f>DEC2HEX(HEX2DEC(B15)+J15)</f>
-        <v>DBF6</v>
+        <v>DCE8</v>
       </c>
       <c r="D15" t="s">
         <v>91</v>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="H15">
         <f>HEX2DEC(RIGHT(E15,2))/2</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I15">
         <f>HEX2DEC(LEFT(E15,2))</f>
@@ -2233,11 +2233,11 @@
       </c>
       <c r="J15">
         <f>H15*I15*2</f>
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DBA8 $3b15 $3b3e ; MST in shop</v>
+        <v xml:space="preserve">  PatchWindow $DC88 $3b15 $3b3e ; MST in shop</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
@@ -2297,7 +2297,7 @@
         <v>88</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -2369,11 +2369,11 @@
       </c>
       <c r="B19" t="str">
         <f>C14</f>
-        <v>DC18</v>
+        <v>DC16</v>
       </c>
       <c r="C19" t="str">
         <f>DEC2HEX(HEX2DEC(B19)+J19)</f>
-        <v>DC48</v>
+        <v>DC46</v>
       </c>
       <c r="D19" t="s">
         <v>30</v>
@@ -2401,7 +2401,7 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DC18 $3015 $3036 ; Active player (during battle)</v>
+        <v xml:space="preserve">  PatchWindow $DC16 $3015 $3036 ; Active player (during battle)</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
@@ -2420,7 +2420,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F20" t="s">
         <v>69</v>
@@ -2532,12 +2532,12 @@
         <v>86</v>
       </c>
       <c r="B23" t="str">
-        <f>C10</f>
-        <v>DBF8</v>
+        <f>C20</f>
+        <v>DF28</v>
       </c>
       <c r="C23" t="str">
         <f>DEC2HEX(HEX2DEC(B23)+J23)</f>
-        <v>DC2A</v>
+        <v>DF5A</v>
       </c>
       <c r="D23" t="s">
         <v>54</v>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="K23" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  PatchWindow $DBF8 $38c1 $38e1 ; Yes/No</v>
+        <v xml:space="preserve">  PatchWindow $DF28 $38c1 $38e1 ; Yes/No</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">

</xml_diff>